<commit_message>
More excel files added
</commit_message>
<xml_diff>
--- a/Football Club Stats.zip_unzipped/Football Club Stats/Liverpool Stats.xlsx
+++ b/Football Club Stats.zip_unzipped/Football Club Stats/Liverpool Stats.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61d616e511083e6c/Documents/Uni/Module 2- Digital Maths and Programming/Uni-Assignment/Uni-Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61d616e511083e6c/Documents/Uni/Module 2- Digital Maths and Programming/Uni-Assignment/Uni-Assignment/Football Club Stats.zip_unzipped/Football Club Stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEB506AA-B7E5-44B4-87AF-4D4A47324DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{5D9687BC-6F32-40D4-BC9B-7C66FFCDBA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0646FAB-EAEE-46E5-B73E-4B49EB06B765}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7D801229-62B4-4D46-8830-14B20E3B73EE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Liverpool Stats" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -133,6 +133,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F3199D6-65AA-43E9-A89B-2666067BF545}" name="Table1" displayName="Table1" ref="A1:M2" totalsRowShown="0">
+  <autoFilter ref="A1:M2" xr:uid="{8F3199D6-65AA-43E9-A89B-2666067BF545}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{DED3592E-E861-4719-A723-D77BA3917D75}" name="Team"/>
+    <tableColumn id="2" xr3:uid="{6DB14081-ECF2-4E9D-B972-21855545A430}" name="Table Position"/>
+    <tableColumn id="3" xr3:uid="{7CCEB19E-03F9-4970-A7ED-6A9F02714D2E}" name="Points"/>
+    <tableColumn id="4" xr3:uid="{85FB9849-E565-4F1C-9043-A74E715FC94D}" name="Matches Played"/>
+    <tableColumn id="5" xr3:uid="{01078EA1-CD48-4D44-A145-67C8F80C1EC6}" name="Wins"/>
+    <tableColumn id="6" xr3:uid="{42A862EC-A0CE-4082-93EB-5F226C686966}" name="Losses"/>
+    <tableColumn id="7" xr3:uid="{3DBCDF86-0305-43F8-840D-3A3F1D969721}" name="Draws"/>
+    <tableColumn id="8" xr3:uid="{9426D573-CFC8-4463-B189-E0972F2D52EE}" name="Goals For"/>
+    <tableColumn id="9" xr3:uid="{F184B122-61EA-477D-86A8-744D0316DE0B}" name="Goals Against"/>
+    <tableColumn id="10" xr3:uid="{AC826E6B-C74B-478E-930A-138D49C875B5}" name="Goal Difference"/>
+    <tableColumn id="11" xr3:uid="{469F3654-C552-4067-B834-67EC3C24FF6E}" name="Top Scorer"/>
+    <tableColumn id="12" xr3:uid="{67E77176-D8D1-48D4-B0DC-6398B9F88118}" name="Red Cards"/>
+    <tableColumn id="13" xr3:uid="{285FB0AE-E27D-4F57-96C7-8763FDB0F179}" name="Yellow Cards"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -454,20 +476,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6337A9-C999-4D55-9232-8E305BBE19B2}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" customWidth="1"/>
+    <col min="12" max="12" width="11.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -554,5 +577,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>